<commit_message>
The Sep-Oct 2020 update
</commit_message>
<xml_diff>
--- a/Leaderboards/ME3MP-TCHOF-DeltaSquad.xlsx
+++ b/Leaderboards/ME3MP-TCHOF-DeltaSquad.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MEHOF\Leaderboards\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3740D5-191C-49DB-A715-09291EF9B2D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C6220A-CE09-4C2B-8040-96C752FBC96F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27885" windowHeight="18240" tabRatio="719" activeTab="2" xr2:uid="{0BA8A437-E564-4296-AF23-437220D626B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="18240" tabRatio="719" activeTab="2" xr2:uid="{0BA8A437-E564-4296-AF23-437220D626B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Player Gold" sheetId="4" r:id="rId1"/>
@@ -22,7 +17,6 @@
     <definedName name="ExternalData_18" localSheetId="3" hidden="1">'Team Platinum'!$C$1:$J$8</definedName>
     <definedName name="ExternalData_19" localSheetId="1" hidden="1">'Team Gold'!$C$1:$F$2</definedName>
     <definedName name="ExternalData_3" localSheetId="0" hidden="1">'Player Gold'!$C$1:$F$5</definedName>
-    <definedName name="ExternalData_4" localSheetId="2" hidden="1">'Player Platinum'!$C$1:$J$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,37 +26,14 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{CC6E3436-E4E6-4A73-BDDF-97D9753EDFDD}" keepAlive="1" name="Query - PlayerGold" description="Connection to the 'PlayerGold' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=PlayerGold;Extended Properties=&quot;&quot;" command="SELECT * FROM [PlayerGold]"/>
-  </connection>
-  <connection id="2" xr16:uid="{ABC27D64-C74F-4333-9FCC-D0B44201D4D8}" keepAlive="1" name="Query - PlayerPlatinum" description="Connection to the 'PlayerPlatinum' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=PlayerPlatinum;Extended Properties=&quot;&quot;" command="SELECT * FROM [PlayerPlatinum]"/>
-  </connection>
-  <connection id="3" xr16:uid="{88EB767B-2A81-4243-AC9C-4E75CAE65C88}" keepAlive="1" name="Query - PlayerRuns" description="Connection to the 'PlayerRuns' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=PlayerRuns;Extended Properties=&quot;&quot;" command="SELECT * FROM [PlayerRuns]"/>
-  </connection>
-  <connection id="4" xr16:uid="{6378C547-362C-4CF1-B899-5C0E5C2B4944}" keepAlive="1" name="Query - RunsByPlayerFilePath" description="Connection to the 'RunsByPlayerFilePath' query in the workbook." type="5" refreshedVersion="0" background="1">
-    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=RunsByPlayerFilePath;Extended Properties=&quot;&quot;" command="SELECT * FROM [RunsByPlayerFilePath]"/>
-  </connection>
-  <connection id="5" xr16:uid="{879FC04E-ABC4-4366-AB4C-63151C995D81}" keepAlive="1" name="Query - TeamGold" description="Connection to the 'TeamGold' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=TeamGold;Extended Properties=&quot;&quot;" command="SELECT * FROM [TeamGold]"/>
-  </connection>
-  <connection id="6" xr16:uid="{82901C82-C7BD-45CE-8155-D3A03E6836A2}" keepAlive="1" name="Query - TeamPlatinum" description="Connection to the 'TeamPlatinum' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=TeamPlatinum;Extended Properties=&quot;&quot;" command="SELECT * FROM [TeamPlatinum]"/>
-  </connection>
-  <connection id="7" xr16:uid="{D6454015-BFA0-4BCC-ACC1-85D282D86E64}" keepAlive="1" name="Query - TeamRuns" description="Connection to the 'TeamRuns' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
-    <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=TeamRuns;Extended Properties=&quot;&quot;" command="SELECT * FROM [TeamRuns]"/>
-  </connection>
-</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -228,15 +199,39 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -249,31 +244,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -309,162 +280,94 @@
 </styleSheet>
 </file>
 
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_3" connectionId="1" xr16:uid="{01D5C563-7914-4119-B277-6E0365AB180C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="39" unboundColumnsLeft="2">
-    <queryTableFields count="6">
-      <queryTableField id="15" dataBound="0" tableColumnId="15"/>
-      <queryTableField id="17" dataBound="0" tableColumnId="16"/>
-      <queryTableField id="2" name="Player" tableColumnId="2"/>
-      <queryTableField id="18" dataBound="0" tableColumnId="17"/>
-      <queryTableField id="33" name="Coruscant terrorist coup" tableColumnId="1"/>
-      <queryTableField id="34" name="Underground Separatist Droid Factory" tableColumnId="3"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_19" connectionId="5" xr16:uid="{8A10293E-1922-4C01-8C87-D43FE7C2D348}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="17" unboundColumnsLeft="2">
-    <queryTableFields count="6">
-      <queryTableField id="5" dataBound="0" tableColumnId="5"/>
-      <queryTableField id="7" dataBound="0" tableColumnId="6"/>
-      <queryTableField id="1" name="Team" tableColumnId="1"/>
-      <queryTableField id="8" dataBound="0" tableColumnId="7"/>
-      <queryTableField id="11" name="Coruscant terrorist coup" tableColumnId="2"/>
-      <queryTableField id="12" name="Underground Separatist Droid Factory" tableColumnId="3"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_4" connectionId="2" xr16:uid="{4FDB064C-9384-40BD-BB83-406C4AAE676C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="44" unboundColumnsLeft="2">
-    <queryTableFields count="10">
-      <queryTableField id="15" dataBound="0" tableColumnId="15"/>
-      <queryTableField id="17" dataBound="0" tableColumnId="16"/>
-      <queryTableField id="2" name="Player" tableColumnId="2"/>
-      <queryTableField id="18" dataBound="0" tableColumnId="17"/>
-      <queryTableField id="33" name="Coruscant terrorist coup" tableColumnId="1"/>
-      <queryTableField id="38" name="Underground Separatist Droid Factory" tableColumnId="7"/>
-      <queryTableField id="37" name="The Ras Prosecutor" tableColumnId="6"/>
-      <queryTableField id="35" name="Kashyyyk Operation" tableColumnId="4"/>
-      <queryTableField id="34" name="Battle for Geonosis" tableColumnId="3"/>
-      <queryTableField id="36" name="Mygeeto" tableColumnId="5"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_18" connectionId="6" xr16:uid="{6685B61A-01C5-405E-BA4F-153036492ECE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="21" unboundColumnsLeft="2">
-    <queryTableFields count="10">
-      <queryTableField id="5" dataBound="0" tableColumnId="5"/>
-      <queryTableField id="7" dataBound="0" tableColumnId="6"/>
-      <queryTableField id="1" name="Team" tableColumnId="1"/>
-      <queryTableField id="8" dataBound="0" tableColumnId="7"/>
-      <queryTableField id="12" name="Coruscant terrorist coup" tableColumnId="3"/>
-      <queryTableField id="16" name="Underground Separatist Droid Factory" tableColumnId="10"/>
-      <queryTableField id="15" name="The Ras Prosecutor" tableColumnId="9"/>
-      <queryTableField id="13" name="Kashyyyk Operation" tableColumnId="4"/>
-      <queryTableField id="11" name="Battle for Geonosis" tableColumnId="2"/>
-      <queryTableField id="14" name="Mygeeto" tableColumnId="8"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{32E75204-A646-44FC-A639-F5D4AA51D1DD}" name="PlayerGold" displayName="PlayerGold" ref="A1:F5" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{32E75204-A646-44FC-A639-F5D4AA51D1DD}" name="PlayerGold" displayName="PlayerGold" ref="A1:F5" totalsRowShown="0">
   <autoFilter ref="A1:F5" xr:uid="{75E32DF2-B7D1-4E21-B067-53EB9F9748A2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F5">
     <sortCondition descending="1" ref="D1:D5"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="15" xr3:uid="{EDDD632F-97A5-450A-A02F-573A672F38AD}" uniqueName="15" name="Time" queryTableFieldId="15" dataDxfId="22">
+    <tableColumn id="15" xr3:uid="{EDDD632F-97A5-450A-A02F-573A672F38AD}" name="Time" dataDxfId="22">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{BEC20656-0D98-41A4-A5E6-592E8E555E2C}" uniqueName="16" name=" - " queryTableFieldId="17" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{109F6945-579B-461B-9EDE-3853C1B22DDB}" uniqueName="2" name="Player" queryTableFieldId="2" dataDxfId="20"/>
-    <tableColumn id="17" xr3:uid="{DC60D44E-66DA-4427-8334-D0AA3B26010B}" uniqueName="17" name="Count" queryTableFieldId="18" dataDxfId="19">
+    <tableColumn id="16" xr3:uid="{BEC20656-0D98-41A4-A5E6-592E8E555E2C}" name=" - " dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{109F6945-579B-461B-9EDE-3853C1B22DDB}" name="Player" dataDxfId="20"/>
+    <tableColumn id="17" xr3:uid="{DC60D44E-66DA-4427-8334-D0AA3B26010B}" name="Count" dataDxfId="19">
       <calculatedColumnFormula>COUNT(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{F01283ED-5023-447B-B4AF-7407570BC001}" uniqueName="1" name="Coruscant terrorist coup" queryTableFieldId="33" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{41A82F62-62ED-4057-856E-DCD55A634B70}" uniqueName="3" name="Underground Separatist Droid Factory" queryTableFieldId="34" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{F01283ED-5023-447B-B4AF-7407570BC001}" name="Coruscant terrorist coup" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{41A82F62-62ED-4057-856E-DCD55A634B70}" name="Underground Separatist Droid Factory" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{B485542F-6500-4DC4-8AA2-D1BF47A40106}" name="TeamGold" displayName="TeamGold" ref="A1:F2" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{B485542F-6500-4DC4-8AA2-D1BF47A40106}" name="TeamGold" displayName="TeamGold" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{CBBCED77-A85B-4C39-A4D8-E08D6648A64A}"/>
   <tableColumns count="6">
-    <tableColumn id="5" xr3:uid="{41E6101F-EED8-4A3E-8AF1-BE36C3773816}" uniqueName="5" name="Time" queryTableFieldId="5" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{41E6101F-EED8-4A3E-8AF1-BE36C3773816}" name="Time" dataDxfId="16">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B4B9613D-6C89-454F-93FC-8D0D60F7149D}" uniqueName="6" name=" - " queryTableFieldId="7" dataDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{CCFF0695-2980-472E-8D1E-D05A801FD794}" uniqueName="1" name="Team" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{51AAD9E0-8DA2-4AA3-9E69-7A9D523AB321}" uniqueName="7" name="Count" queryTableFieldId="8" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{B4B9613D-6C89-454F-93FC-8D0D60F7149D}" name=" - " dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{CCFF0695-2980-472E-8D1E-D05A801FD794}" name="Team" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{51AAD9E0-8DA2-4AA3-9E69-7A9D523AB321}" name="Count" dataDxfId="13">
       <calculatedColumnFormula>COUNT(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C2D86276-5252-4929-A7D1-FDA7BB87092D}" uniqueName="2" name="Coruscant terrorist coup" queryTableFieldId="11" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{7C1F95B0-BEFA-412C-A270-7BDB1C1BA9F3}" uniqueName="3" name="Underground Separatist Droid Factory" queryTableFieldId="12" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{C2D86276-5252-4929-A7D1-FDA7BB87092D}" name="Coruscant terrorist coup" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{7C1F95B0-BEFA-412C-A270-7BDB1C1BA9F3}" name="Underground Separatist Droid Factory" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4D96F15E-13F5-40C3-8F2D-F859F1B7C75E}" name="PlayerPlatinum" displayName="PlayerPlatinum" ref="A1:J16" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4D96F15E-13F5-40C3-8F2D-F859F1B7C75E}" name="PlayerPlatinum" displayName="PlayerPlatinum" ref="A1:J16" totalsRowShown="0">
   <autoFilter ref="A1:J16" xr:uid="{CEEC556E-CD08-4DF7-9BFF-F998BB68785C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J16">
     <sortCondition descending="1" ref="D1:D16"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="15" xr3:uid="{3C88E12B-A717-40A4-9D08-10F2C1C325E7}" uniqueName="15" name="Time" queryTableFieldId="15" dataDxfId="2">
+    <tableColumn id="15" xr3:uid="{3C88E12B-A717-40A4-9D08-10F2C1C325E7}" name="Time" dataDxfId="10">
       <calculatedColumnFormula>SUM(PlayerPlatinum[[#This Row],[Coruscant terrorist coup]:[Mygeeto]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{EC9350BA-7A1A-46DA-89AF-028B9B6306F3}" uniqueName="16" name=" - " queryTableFieldId="17" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{FCBF7C60-BAE4-4F64-8EE1-077CE660D26C}" uniqueName="2" name="Player" queryTableFieldId="2" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{3B739F4F-4398-4D60-A365-8F75C789E22A}" uniqueName="17" name="Count" queryTableFieldId="18" dataDxfId="3">
+    <tableColumn id="16" xr3:uid="{EC9350BA-7A1A-46DA-89AF-028B9B6306F3}" name=" - " dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{FCBF7C60-BAE4-4F64-8EE1-077CE660D26C}" name="Player" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{3B739F4F-4398-4D60-A365-8F75C789E22A}" name="Count" dataDxfId="7">
       <calculatedColumnFormula>COUNT(PlayerPlatinum[[#This Row],[Coruscant terrorist coup]:[Mygeeto]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{15CD3909-DF28-4D86-8C93-0FAF4F345BB6}" uniqueName="1" name="Coruscant terrorist coup" queryTableFieldId="33" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{D5BCFFA6-26BA-40D1-89D3-E3D8D8342FF5}" uniqueName="7" name="Underground Separatist Droid Factory" queryTableFieldId="38"/>
-    <tableColumn id="6" xr3:uid="{AD960240-4182-4A11-8296-6777E7BF8591}" uniqueName="6" name="The Ras Prosecutor" queryTableFieldId="37"/>
-    <tableColumn id="4" xr3:uid="{29FE51E1-C087-4110-9432-019EA0BE821A}" uniqueName="4" name="Kashyyyk Operation" queryTableFieldId="35"/>
-    <tableColumn id="3" xr3:uid="{5DD5FEE7-9203-4E3A-A92E-9838A4B989B4}" uniqueName="3" name="Battle for Geonosis" queryTableFieldId="34"/>
-    <tableColumn id="5" xr3:uid="{289AEAFF-97C0-47A2-9AE0-9ED377C130E6}" uniqueName="5" name="Mygeeto" queryTableFieldId="36"/>
+    <tableColumn id="1" xr3:uid="{15CD3909-DF28-4D86-8C93-0FAF4F345BB6}" name="Coruscant terrorist coup" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{D5BCFFA6-26BA-40D1-89D3-E3D8D8342FF5}" name="Underground Separatist Droid Factory"/>
+    <tableColumn id="6" xr3:uid="{AD960240-4182-4A11-8296-6777E7BF8591}" name="The Ras Prosecutor"/>
+    <tableColumn id="4" xr3:uid="{29FE51E1-C087-4110-9432-019EA0BE821A}" name="Kashyyyk Operation"/>
+    <tableColumn id="3" xr3:uid="{5DD5FEE7-9203-4E3A-A92E-9838A4B989B4}" name="Battle for Geonosis"/>
+    <tableColumn id="5" xr3:uid="{289AEAFF-97C0-47A2-9AE0-9ED377C130E6}" name="Mygeeto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{9335664B-6A7F-41AA-9EC7-B1CD79248B09}" name="TeamPlatinum" displayName="TeamPlatinum" ref="A1:J8" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{9335664B-6A7F-41AA-9EC7-B1CD79248B09}" name="TeamPlatinum" displayName="TeamPlatinum" ref="A1:J8" totalsRowShown="0">
   <autoFilter ref="A1:J8" xr:uid="{2D15F030-F6FF-44A9-A144-BCB443C2214D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J8">
     <sortCondition descending="1" ref="D1:D8"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{5F3E86AB-DA66-4604-910E-DE0EF12B893E}" uniqueName="5" name="Time" queryTableFieldId="5" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{5F3E86AB-DA66-4604-910E-DE0EF12B893E}" name="Time" dataDxfId="5">
       <calculatedColumnFormula>SUM(TeamPlatinum[[#This Row],[Coruscant terrorist coup]:[Mygeeto]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{42F25FBA-F7CF-4F07-8335-FEF145EF13EE}" uniqueName="6" name=" - " queryTableFieldId="7" dataDxfId="16"/>
-    <tableColumn id="1" xr3:uid="{55DD4C52-68B9-4E1E-A984-325F63C84092}" uniqueName="1" name="Team" queryTableFieldId="1" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{53689E7F-6231-4192-9B64-958E1466055D}" uniqueName="7" name="Count" queryTableFieldId="8" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{42F25FBA-F7CF-4F07-8335-FEF145EF13EE}" name=" - " dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{55DD4C52-68B9-4E1E-A984-325F63C84092}" name="Team" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{53689E7F-6231-4192-9B64-958E1466055D}" name="Count" dataDxfId="2">
       <calculatedColumnFormula>COUNT(TeamPlatinum[[#This Row],[Coruscant terrorist coup]:[Mygeeto]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{735C1165-5239-46ED-AEA9-9BA6EE1896FB}" uniqueName="3" name="Coruscant terrorist coup" queryTableFieldId="12" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{CE171A66-F205-49D0-82C0-9057BC0B6A0F}" uniqueName="10" name="Underground Separatist Droid Factory" queryTableFieldId="16"/>
-    <tableColumn id="9" xr3:uid="{53614151-A4BE-4756-BA93-167FF142A306}" uniqueName="9" name="The Ras Prosecutor" queryTableFieldId="15"/>
-    <tableColumn id="4" xr3:uid="{080264A4-9971-47BB-93CF-FCA8B8C50036}" uniqueName="4" name="Kashyyyk Operation" queryTableFieldId="13"/>
-    <tableColumn id="2" xr3:uid="{D68D38D6-EAAF-44A5-9946-3198539F746F}" uniqueName="2" name="Battle for Geonosis" queryTableFieldId="11" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{4A335BBF-4A10-4B3B-924F-3108AD332AB8}" uniqueName="8" name="Mygeeto" queryTableFieldId="14"/>
+    <tableColumn id="3" xr3:uid="{735C1165-5239-46ED-AEA9-9BA6EE1896FB}" name="Coruscant terrorist coup" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{CE171A66-F205-49D0-82C0-9057BC0B6A0F}" name="Underground Separatist Droid Factory"/>
+    <tableColumn id="9" xr3:uid="{53614151-A4BE-4756-BA93-167FF142A306}" name="The Ras Prosecutor"/>
+    <tableColumn id="4" xr3:uid="{080264A4-9971-47BB-93CF-FCA8B8C50036}" name="Kashyyyk Operation"/>
+    <tableColumn id="2" xr3:uid="{D68D38D6-EAAF-44A5-9946-3198539F746F}" name="Battle for Geonosis" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{4A335BBF-4A10-4B3B-924F-3108AD332AB8}" name="Mygeeto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>